<commit_message>
Clean up XLSX sample
</commit_message>
<xml_diff>
--- a/video/tools/import/schedule.xlsx
+++ b/video/tools/import/schedule.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -49,96 +49,10 @@
     <t xml:space="preserve">Room ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Begrüßung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oh je, Java ist nicht mehr kostenlos – und nun?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle hat sein Lizenzmodell geändert, ab JDK 11 kann es in Produktion nicht mehr kostenfrei eingesetzt werden. Seit Januar 2019 gibt es zudem keine freien Updates mehr für Oracles JDK 8. Was sind die Alternativen und wann ergibt der Einsatz welcher JDK-Version Sinn?
-Wir werfen einen Blick auf die Kosten für das Oracle JDK, auf die Preismodelle von anderen kommerziellen Anbietern sowie auf die freien Versionen. Wir diskutieren weiterhin, ob man bei Java 8 bleiben oder auf 11 beziehungsweise das aktuellste JDK-Release wechseln sollte und welche Konsequenzen das mit sich bringt. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eine Reise durch die JDKs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viele von Euch, so wie ich, arbeiten im Job noch mit JDK 8. Daher möchte ich Euch mitnehmen auf die Reise durch die JDKs. Wir starten unsere Reise bei JDK 8 und wandern bis zur aktuellen Version. Außerdem wagen wir einen Blick auf die Attraktionen der zukünftigen Versionen. Wir halten unter anderem an folgenden Stationen:
-- Jshell
-- Private Methods in Interfaces
-- Optional class
-- Schlüsselwort "var"
-- Erweiterung der Collections
-- HttpClient/HttpRequest neues FluentAPI
-- Switch Expressions
-- Erweiterung der String-Klasse
-Diese werden zum Teil anhand von Quelltext-Beispielen veranschaulicht. Ich wünsche Euch eine gute Reise.
-P.S.: Bringt festes Schuhwerk mit. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Java und die GraalVM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die GraalVM ist eine universelle virtuelle Maschine (VM) für Anwendungen, die in JavaScript, Python, Ruby, R oder mit den JVM-basierten Programmiersprachen Java, Scala, Kotlin, Clojure und LLVM-basierten Sprachen wie C/C++ geschrieben wurden. Im August 2020 wird die GraalVM 20.2 freigegeben, mit Performance-Verbesserungen und polyglotter Unterstützung für verschiedene Programmiersprachen. Sie ermöglicht damit die Interoperabilität in einer gemeinsamen Laufzeitumgebung. GraalVM kann eigenständig oder im Kontext von OpenJDK, Node.js, Oracle-Datenbank oder MySQL betrieben werden.
-Mit GraalVMs Ahead-of-Time-Fähigkeit kompilierte Native Images verfügen über eine optimierte Start-up-Zeit und sie verringern den Memory-Verbrauch von JVM-basierten Applikationen. Die GraalVM kann wahlweise als Open Source Community Edition (CE) oder als Enterprise Edition (EE) mit OTN-Lizenz verwendet werden.
-Im Vortrag wird die GraalVM-Architektur im Java-Ökosystem dargestellt und die Einsatzgebiete werden erläutert, beispielsweise der in Java entwickelte C2 JIT Compiler oder die Verwendung von GraalVM Native Images. GraalVM und OpenJDK können auch für Microservices-Frameworks verwendet werden. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WW</t>
+    <t xml:space="preserve">External URL</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mittagspause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclipse MicroProfile – der Java-Standard für die Cloud </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Java Enterprise Edition hat sich über zwei Jahrzehnte entwickelt, um verteilte Anwendungen zu betreiben. Mit dem MicroProfile beginnt ein Reload von Java EE für Microservices und die Cloud. Bestehende Standards von Java EE werden weiter verwendet oder auch aussortiert. Neue Standards werden aufgenommen. 
-Mit der bald erscheinenden Version 4.0 ist das MicroProfile mehr als erwachsen geworden. Fast zeitgleich wird Jakarta EE in Version 9 erscheinen. Hier lohnt sich ein Blick, wie und ob diese beiden Standards miteinander interagieren und in Beziehung stehen. Das Hauptziel wird es aber sein, das Eclipse MicroProfile und seine einzelnen Teile kennenzulernen. Beispielhaft seien hier nur einige genannt, angefangen von Config, Health, Opentracing, Open-Api, Fault-Tolerance und vieles andere mehr. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloud-native Java mit Quarkus und MicroProfile </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Innovationskraft der Java-Welt ist ungebrochen: Noch immer werden regelmäßig höchst interessante neue Projekte vorgestellt. Dieser praxisnahe Talk beleuchtet, wie zwei solche Projekte miteinander kombiniert werden können, um zeitgemäße Anwendungen für die Cloud zu entwickeln. MicroProfile bietet eine ganze Reihe nützlicher APIs für Cloud-basierte Anwendungen. Hierzu zählen die Unterstützung von Fault Tolerance, Open API, Health Checks, Metrics und Open Tracing. Mit Hilfe von Quarkus (und der GraalVM) werden daraus native Anwendungen, die innerhalb von Millisekunden starten und einen extrem kleinen Speicherverbrauch haben. Eine Beispielanwendung wird während des Talks live erstellt. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software-Modularisierung – aber wie? Empfehlungen mit und gegen den Trend </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software-Architektur ist zunächst etwas sehr Einfaches: Wir definieren klar abgegrenzte Bausteine und die Beziehungen zwischen diesen Bausteinen. Das war's. Mit etwas Mühe lassen sich in jeder Anwendung fachliche Schnitte finden, um die geforderten Bausteine voneinander abzugrenzen. Doch welche Modularisierungstechnik sollte man dabei wählen? Java Package? JAR? Jigsaw Modul? OSGI Bundle? ReSTful API? Microservice? Docker-Container? Kubernetes Pod? 
-In dieser Session möchte Thorsten Teilnehmerinnen und Teilnehmer ermutigen, Entscheidungen im Zweifel auch gegen den aktuellen Markthype und für die zu ihren Anforderungen passende Technik zu treffen. Dazu berichtet er über unsere selbst gemachten Erfahrungen. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It's a match: Kotlin, Micronaut und GraalVM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das JVM-Framework Micronaut entwickelt sich zunehmend als Konkurrenz zum etablierten Spring Boot. Unter anderem deshalb, weil es das leistungsstarke und dennoch schlanke Framework schafft, Startzeit und Speicherverbrauch erheblich zu reduzieren. Dies macht es nicht nur für die Entwicklung containerisierter Microservices interessant, sondern auch für Serverless Computing. 
-Aber auch die Unterstützung von Kotlin als first-class Language – neben Java und Groovy – trägt zum Erfolg bei, finden doch immer mehr Entwickler Gefallen an der effizienten Java-Alternative. Zudem vereinfacht Micronaut die Entwicklung für Oracles GraalVM. Diese ermöglicht das Erzeugen nativer Images, die Startzeit und Speicherverbrauch nochmals senken. 
-Der Vortrag umfasst eine Einführung in Micronaut. Dazu wird – nach einer Vorstellung der grundlegenden Technologien – live ein Microservice mit Kotlin und Micronaut codiert. Anschließend wird der Service per GraalVM als natives Binary kompiliert. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS</t>
   </si>
   <si>
     <t xml:space="preserve">How to fill in this spreadsheet</t>
@@ -162,55 +76,10 @@
     <t xml:space="preserve">Avatar</t>
   </si>
   <si>
-    <t xml:space="preserve">Falk Sippach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12143_1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandra Geberding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12111_1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wolfgang Weigend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12024_1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sascha Groß</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12145_1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thilo Frotscher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12192_1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thorsten Maier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12141_1.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Keep the speaker IDs consistent between updates</t>
   </si>
   <si>
-    <t xml:space="preserve">Christian Schwörer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.herbstcampus.de/common/images/numbers/12353_1.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">- The avatar should be a URL to an image, but can be left blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hörsaal „Nürnberg“</t>
   </si>
   <si>
     <t xml:space="preserve">- Keep the room IDs consistent between updates</t>
@@ -622,7 +491,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="room_id" displayName="room_id" ref="A2:A1048576" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" name="H"/>
+    <tableColumn id="1" name=""/>
   </tableColumns>
 </table>
 </file>
@@ -645,10 +514,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.72"/>
@@ -685,223 +554,64 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>44076.375</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>44076.3854166667</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>44076.3854166667</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>44076.4166666667</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>44076.4270833333</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>44076.4583333333</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="5"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="5"/>
+      <c r="H4" s="4"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>44076.46875</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>44076.5</v>
-      </c>
-      <c r="H5" s="4" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="L5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>44076.5</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>44076.5416666667</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="H6" s="4"/>
       <c r="J6" s="9"/>
       <c r="K6" s="12" t="n">
         <v>1</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>44076.5416666667</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>44076.5729166667</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="5"/>
+      <c r="H7" s="4"/>
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
       <c r="L7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>44076.5833333333</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>44076.6145833333</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>44076.625</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>44076.65625</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="5"/>
+      <c r="H9" s="4"/>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>44076.6666666667</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>44076.6979166667</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="5"/>
+      <c r="H10" s="4"/>
       <c r="L10" s="19"/>
       <c r="M10" s="20" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="N10" s="21"/>
     </row>
@@ -915,7 +625,7 @@
       <c r="H12" s="4"/>
       <c r="L12" s="19"/>
       <c r="M12" s="22" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="N12" s="21"/>
     </row>
@@ -923,7 +633,7 @@
       <c r="H13" s="4"/>
       <c r="L13" s="19"/>
       <c r="M13" s="22" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="N13" s="21"/>
     </row>
@@ -931,7 +641,7 @@
       <c r="H14" s="4"/>
       <c r="L14" s="19"/>
       <c r="M14" s="22" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="N14" s="21"/>
     </row>
@@ -939,7 +649,7 @@
       <c r="H15" s="4"/>
       <c r="L15" s="19"/>
       <c r="M15" s="22" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="N15" s="21"/>
     </row>
@@ -3984,10 +3694,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="80.71"/>
@@ -3999,107 +3709,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="E5" s="19"/>
       <c r="F5" s="20" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="19"/>
       <c r="F6" s="22"/>
       <c r="G6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="19"/>
       <c r="F7" s="22" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="G7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="E8" s="19"/>
       <c r="F8" s="22" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="G8" s="21"/>
     </row>
@@ -4129,10 +3772,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.64"/>
@@ -4144,15 +3787,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4163,7 +3798,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="19"/>
       <c r="E5" s="20" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F5" s="21"/>
     </row>
@@ -4175,14 +3810,14 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="19"/>
       <c r="E7" s="22" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="19"/>
       <c r="E8" s="22" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="F8" s="21"/>
     </row>
@@ -4218,7 +3853,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.81"/>
@@ -4230,10 +3865,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4244,7 +3879,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="19"/>
       <c r="F5" s="20" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G5" s="21"/>
     </row>
@@ -4256,21 +3891,21 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="19"/>
       <c r="F7" s="22" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="G7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="19"/>
       <c r="F8" s="22" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="G8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="G9" s="21"/>
     </row>

</xml_diff>

<commit_message>
Improvements to import script
</commit_message>
<xml_diff>
--- a/video/tools/import/schedule.xlsx
+++ b/video/tools/import/schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Talks" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biography</t>
   </si>
   <si>
     <t xml:space="preserve">- Keep the speaker IDs consistent between updates</t>
@@ -511,13 +514,13 @@
   </sheetPr>
   <dimension ref="A1:N1016"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.72"/>
@@ -3691,13 +3694,13 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="80.71"/>
@@ -3714,6 +3717,9 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="16"/>
@@ -3735,14 +3741,14 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="19"/>
       <c r="F7" s="22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="19"/>
       <c r="F8" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="21"/>
     </row>
@@ -3775,7 +3781,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.64"/>
@@ -3810,14 +3816,14 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="19"/>
       <c r="E7" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="19"/>
       <c r="E8" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="21"/>
     </row>
@@ -3853,7 +3859,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.81"/>
@@ -3868,7 +3874,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,21 +3897,21 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="19"/>
       <c r="F7" s="22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="19"/>
       <c r="F8" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="21"/>
     </row>

</xml_diff>